<commit_message>
Upload from 2015_03_22 email from Thomas Martin
</commit_message>
<xml_diff>
--- a/data/raw/FormattedArchaealMetadata.xlsx
+++ b/data/raw/FormattedArchaealMetadata.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25516"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="14800" windowHeight="8020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -408,7 +413,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -443,7 +448,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -658,16 +663,16 @@
       <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="14" max="14" width="25.42578125" customWidth="1"/>
-    <col min="19" max="19" width="37.5703125" customWidth="1"/>
+    <col min="14" max="14" width="67.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="37.5" customWidth="1"/>
     <col min="21" max="21" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -759,7 +764,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30">
       <c r="A2">
         <v>2264867065</v>
       </c>
@@ -785,7 +790,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="A3">
         <v>2264867072</v>
       </c>
@@ -811,7 +816,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30">
       <c r="A4">
         <v>2524023115</v>
       </c>
@@ -840,7 +845,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5">
         <v>2524023065</v>
       </c>
@@ -860,7 +865,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6">
         <v>2576861416</v>
       </c>
@@ -880,7 +885,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7">
         <v>2519103050</v>
       </c>
@@ -906,7 +911,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8">
         <v>2524023120</v>
       </c>
@@ -935,7 +940,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9">
         <v>2574179760</v>
       </c>
@@ -955,7 +960,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10">
         <v>2523533574</v>
       </c>
@@ -975,7 +980,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11">
         <v>2264867224</v>
       </c>
@@ -1004,7 +1009,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30">
       <c r="A12">
         <v>2576861411</v>
       </c>
@@ -1024,7 +1029,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30">
       <c r="A13">
         <v>2264867002</v>
       </c>
@@ -1053,7 +1058,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30">
       <c r="A14">
         <v>2264867000</v>
       </c>
@@ -1082,7 +1087,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30">
       <c r="A15">
         <v>2576861415</v>
       </c>
@@ -1102,7 +1107,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30">
       <c r="A16">
         <v>2576861414</v>
       </c>
@@ -1122,7 +1127,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28">
       <c r="A17">
         <v>2264867226</v>
       </c>
@@ -1151,7 +1156,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28">
       <c r="A18">
         <v>2524614574</v>
       </c>
@@ -1171,7 +1176,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28">
       <c r="A19">
         <v>2518645523</v>
       </c>
@@ -1200,7 +1205,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28">
       <c r="A20">
         <v>2576861417</v>
       </c>
@@ -1220,7 +1225,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28">
       <c r="A21">
         <v>2517572171</v>
       </c>
@@ -1249,7 +1254,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28">
       <c r="A22">
         <v>2264867063</v>
       </c>
@@ -1275,7 +1280,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28">
       <c r="A23">
         <v>2264867027</v>
       </c>
@@ -1295,7 +1300,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28">
       <c r="A24">
         <v>2264867003</v>
       </c>
@@ -1324,7 +1329,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28">
       <c r="A25">
         <v>2527291500</v>
       </c>
@@ -1353,7 +1358,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28">
       <c r="A26">
         <v>2524023105</v>
       </c>
@@ -1382,7 +1387,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28">
       <c r="A27">
         <v>2517572169</v>
       </c>
@@ -1411,7 +1416,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28">
       <c r="A28">
         <v>2527291507</v>
       </c>
@@ -1440,7 +1445,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28">
       <c r="A29">
         <v>2522572163</v>
       </c>
@@ -1460,7 +1465,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28">
       <c r="A30">
         <v>2264867248</v>
       </c>
@@ -1486,7 +1491,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28">
       <c r="A31">
         <v>2576861413</v>
       </c>
@@ -1506,7 +1511,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28">
       <c r="A32">
         <v>2527291513</v>
       </c>
@@ -1535,7 +1540,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28">
       <c r="A33">
         <v>2264867067</v>
       </c>
@@ -1561,7 +1566,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28">
       <c r="A34">
         <v>2527291512</v>
       </c>
@@ -1590,7 +1595,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28">
       <c r="A35">
         <v>2264867066</v>
       </c>
@@ -1616,7 +1621,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28">
       <c r="A36">
         <v>2529292698</v>
       </c>
@@ -1642,7 +1647,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28">
       <c r="A37">
         <v>2264867218</v>
       </c>
@@ -1671,7 +1676,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28">
       <c r="A38">
         <v>2524614572</v>
       </c>
@@ -1691,7 +1696,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28">
       <c r="A39">
         <v>2527291509</v>
       </c>
@@ -1720,7 +1725,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28">
       <c r="A40">
         <v>2527291506</v>
       </c>
@@ -1746,7 +1751,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28">
       <c r="A41">
         <v>2264867064</v>
       </c>
@@ -1775,7 +1780,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28">
       <c r="A42">
         <v>2517572170</v>
       </c>
@@ -1804,7 +1809,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28">
       <c r="A43">
         <v>2517572172</v>
       </c>
@@ -1833,7 +1838,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28">
       <c r="A44">
         <v>2264867070</v>
       </c>
@@ -1859,7 +1864,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28">
       <c r="A45">
         <v>2264867069</v>
       </c>
@@ -1890,5 +1895,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update from Rene's 5/28 email
</commit_message>
<xml_diff>
--- a/data/raw/FormattedArchaealMetadata.xlsx
+++ b/data/raw/FormattedArchaealMetadata.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25915"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="14800" windowHeight="8020"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="24800" windowHeight="14500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="121">
   <si>
     <t>host</t>
   </si>
@@ -316,16 +316,98 @@
   </si>
   <si>
     <t>habitat_slv</t>
+  </si>
+  <si>
+    <t>agriculture</t>
+  </si>
+  <si>
+    <t>marine</t>
+  </si>
+  <si>
+    <t>surface</t>
+  </si>
+  <si>
+    <t>vertebrate</t>
+  </si>
+  <si>
+    <t>pollution</t>
+  </si>
+  <si>
+    <t>desert</t>
+  </si>
+  <si>
+    <t>fresh</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>arthopod</t>
+  </si>
+  <si>
+    <t>industrial/mining</t>
+  </si>
+  <si>
+    <t>BI</t>
+  </si>
+  <si>
+    <t>Bi</t>
+  </si>
+  <si>
+    <t>AqM</t>
+  </si>
+  <si>
+    <t>AqH</t>
+  </si>
+  <si>
+    <t>Aqm</t>
+  </si>
+  <si>
+    <t>Aqh</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>770m</t>
+  </si>
+  <si>
+    <t>Marine Group I crenarchaeote sp. SCGC</t>
+  </si>
+  <si>
+    <t>HOT station ALOHA, North Pacific Sub-Tropical Gyre</t>
+  </si>
+  <si>
+    <t>Marine Group I crenarchaeote sp. SCGC AAA288-I14</t>
+  </si>
+  <si>
+    <t>Marine Group III euryarchaeote sp. SCGC AAA288-E19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -348,13 +430,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -657,11 +747,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD45"/>
+  <dimension ref="A1:AL47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -672,7 +760,7 @@
     <col min="21" max="21" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -763,8 +851,11 @@
       <c r="AD1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:30">
+      <c r="AE1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31">
       <c r="A2">
         <v>2264867065</v>
       </c>
@@ -789,8 +880,11 @@
       <c r="AB2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="3" spans="1:30">
+      <c r="AE2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31">
       <c r="A3">
         <v>2264867072</v>
       </c>
@@ -815,8 +909,11 @@
       <c r="AB3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="4" spans="1:30">
+      <c r="AE3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31">
       <c r="A4">
         <v>2524023115</v>
       </c>
@@ -844,8 +941,11 @@
       <c r="AB4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="5" spans="1:30">
+      <c r="AE4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31">
       <c r="A5">
         <v>2524023065</v>
       </c>
@@ -864,8 +964,11 @@
       <c r="AB5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="6" spans="1:30">
+      <c r="AE5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31">
       <c r="A6">
         <v>2576861416</v>
       </c>
@@ -884,8 +987,11 @@
       <c r="AB6" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="7" spans="1:30">
+      <c r="AE6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31">
       <c r="A7">
         <v>2519103050</v>
       </c>
@@ -910,8 +1016,11 @@
       <c r="AB7" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="8" spans="1:30">
+      <c r="AE7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31">
       <c r="A8">
         <v>2524023120</v>
       </c>
@@ -939,8 +1048,11 @@
       <c r="AB8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="9" spans="1:30">
+      <c r="AE8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31">
       <c r="A9">
         <v>2574179760</v>
       </c>
@@ -959,8 +1071,11 @@
       <c r="AB9" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="10" spans="1:30">
+      <c r="AE9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31">
       <c r="A10">
         <v>2523533574</v>
       </c>
@@ -979,8 +1094,11 @@
       <c r="AB10" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="11" spans="1:30">
+      <c r="AE10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31">
       <c r="A11">
         <v>2264867224</v>
       </c>
@@ -1008,8 +1126,11 @@
       <c r="AB11" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="12" spans="1:30">
+      <c r="AE11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31">
       <c r="A12">
         <v>2576861411</v>
       </c>
@@ -1028,8 +1149,11 @@
       <c r="AB12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="13" spans="1:30">
+      <c r="AE12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31">
       <c r="A13">
         <v>2264867002</v>
       </c>
@@ -1057,8 +1181,11 @@
       <c r="AB13" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="14" spans="1:30">
+      <c r="AE13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31">
       <c r="A14">
         <v>2264867000</v>
       </c>
@@ -1086,8 +1213,11 @@
       <c r="AB14" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="15" spans="1:30">
+      <c r="AE14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31">
       <c r="A15">
         <v>2576861415</v>
       </c>
@@ -1106,8 +1236,11 @@
       <c r="AB15" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="16" spans="1:30">
+      <c r="AE15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31">
       <c r="A16">
         <v>2576861414</v>
       </c>
@@ -1126,8 +1259,11 @@
       <c r="AB16" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="17" spans="1:28">
+      <c r="AE16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31">
       <c r="A17">
         <v>2264867226</v>
       </c>
@@ -1155,8 +1291,11 @@
       <c r="AB17" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="18" spans="1:28">
+      <c r="AE17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31">
       <c r="A18">
         <v>2524614574</v>
       </c>
@@ -1175,8 +1314,11 @@
       <c r="AB18" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="19" spans="1:28">
+      <c r="AE18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31">
       <c r="A19">
         <v>2518645523</v>
       </c>
@@ -1204,8 +1346,11 @@
       <c r="AB19" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="20" spans="1:28">
+      <c r="AE19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31">
       <c r="A20">
         <v>2576861417</v>
       </c>
@@ -1224,8 +1369,11 @@
       <c r="AB20" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="21" spans="1:28">
+      <c r="AE20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31">
       <c r="A21">
         <v>2517572171</v>
       </c>
@@ -1253,8 +1401,11 @@
       <c r="AB21" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="22" spans="1:28">
+      <c r="AE21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31">
       <c r="A22">
         <v>2264867063</v>
       </c>
@@ -1279,8 +1430,11 @@
       <c r="AB22" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="23" spans="1:28">
+      <c r="AE22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31">
       <c r="A23">
         <v>2264867027</v>
       </c>
@@ -1299,8 +1453,11 @@
       <c r="AB23" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="24" spans="1:28">
+      <c r="AE23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31">
       <c r="A24">
         <v>2264867003</v>
       </c>
@@ -1328,8 +1485,11 @@
       <c r="AB24" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="25" spans="1:28">
+      <c r="AE24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31">
       <c r="A25">
         <v>2527291500</v>
       </c>
@@ -1357,8 +1517,11 @@
       <c r="AB25" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="26" spans="1:28">
+      <c r="AE25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31">
       <c r="A26">
         <v>2524023105</v>
       </c>
@@ -1386,8 +1549,11 @@
       <c r="AB26" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="27" spans="1:28">
+      <c r="AE26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31">
       <c r="A27">
         <v>2517572169</v>
       </c>
@@ -1415,8 +1581,11 @@
       <c r="AB27" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="28" spans="1:28">
+      <c r="AE27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31">
       <c r="A28">
         <v>2527291507</v>
       </c>
@@ -1444,8 +1613,11 @@
       <c r="AB28" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="29" spans="1:28">
+      <c r="AE28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31">
       <c r="A29">
         <v>2522572163</v>
       </c>
@@ -1464,8 +1636,11 @@
       <c r="AB29" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="30" spans="1:28">
+      <c r="AE29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31">
       <c r="A30">
         <v>2264867248</v>
       </c>
@@ -1490,8 +1665,11 @@
       <c r="AB30" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="31" spans="1:28">
+      <c r="AE30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31">
       <c r="A31">
         <v>2576861413</v>
       </c>
@@ -1510,8 +1688,11 @@
       <c r="AB31" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="32" spans="1:28">
+      <c r="AE31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31">
       <c r="A32">
         <v>2527291513</v>
       </c>
@@ -1539,8 +1720,11 @@
       <c r="AB32" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="33" spans="1:28">
+      <c r="AE32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:38">
       <c r="A33">
         <v>2264867067</v>
       </c>
@@ -1565,8 +1749,11 @@
       <c r="AB33" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="34" spans="1:28">
+      <c r="AE33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:38">
       <c r="A34">
         <v>2527291512</v>
       </c>
@@ -1594,8 +1781,11 @@
       <c r="AB34" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="35" spans="1:28">
+      <c r="AE34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:38">
       <c r="A35">
         <v>2264867066</v>
       </c>
@@ -1620,8 +1810,11 @@
       <c r="AB35" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="36" spans="1:28">
+      <c r="AE35" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:38">
       <c r="A36">
         <v>2529292698</v>
       </c>
@@ -1646,8 +1839,11 @@
       <c r="AB36" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="37" spans="1:28">
+      <c r="AE36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:38">
       <c r="A37">
         <v>2264867218</v>
       </c>
@@ -1675,8 +1871,11 @@
       <c r="AB37" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="38" spans="1:28">
+      <c r="AE37" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:38">
       <c r="A38">
         <v>2524614572</v>
       </c>
@@ -1695,8 +1894,11 @@
       <c r="AB38" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="39" spans="1:28">
+      <c r="AE38" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:38">
       <c r="A39">
         <v>2527291509</v>
       </c>
@@ -1724,8 +1926,11 @@
       <c r="AB39" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="40" spans="1:28">
+      <c r="AE39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:38">
       <c r="A40">
         <v>2527291506</v>
       </c>
@@ -1750,8 +1955,11 @@
       <c r="AB40" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="41" spans="1:28">
+      <c r="AE40" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:38">
       <c r="A41">
         <v>2264867064</v>
       </c>
@@ -1779,8 +1987,11 @@
       <c r="AB41" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="42" spans="1:28">
+      <c r="AE41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:38">
       <c r="A42">
         <v>2517572170</v>
       </c>
@@ -1808,8 +2019,11 @@
       <c r="AB42" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="43" spans="1:28">
+      <c r="AE42" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:38">
       <c r="A43">
         <v>2517572172</v>
       </c>
@@ -1837,8 +2051,11 @@
       <c r="AB43" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="44" spans="1:28">
+      <c r="AE43" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:38">
       <c r="A44">
         <v>2264867070</v>
       </c>
@@ -1863,8 +2080,11 @@
       <c r="AB44" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="45" spans="1:28">
+      <c r="AE44" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:38">
       <c r="A45">
         <v>2264867069</v>
       </c>
@@ -1892,9 +2112,115 @@
       <c r="AB45" t="s">
         <v>92</v>
       </c>
+      <c r="AE45" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:38">
+      <c r="A46">
+        <v>2263328039</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1</v>
+      </c>
+      <c r="H46" t="s">
+        <v>26</v>
+      </c>
+      <c r="N46" t="s">
+        <v>120</v>
+      </c>
+      <c r="P46" t="s">
+        <v>1</v>
+      </c>
+      <c r="S46" t="s">
+        <v>118</v>
+      </c>
+      <c r="U46" t="s">
+        <v>82</v>
+      </c>
+      <c r="V46" s="2"/>
+      <c r="W46" s="1"/>
+      <c r="X46" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH46" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI46" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ46" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK46" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL46" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:38">
+      <c r="A47">
+        <v>2513237066</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1</v>
+      </c>
+      <c r="H47" t="s">
+        <v>26</v>
+      </c>
+      <c r="N47" t="s">
+        <v>119</v>
+      </c>
+      <c r="P47" t="s">
+        <v>1</v>
+      </c>
+      <c r="S47" t="s">
+        <v>118</v>
+      </c>
+      <c r="U47" t="s">
+        <v>82</v>
+      </c>
+      <c r="X47" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC47" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE47" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH47" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI47" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ47" t="s">
+        <v>106</v>
+      </c>
+      <c r="AK47" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL47" t="s">
+        <v>108</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Remove extra columns as the end of sheet
</commit_message>
<xml_diff>
--- a/data/raw/FormattedArchaealMetadata.xlsx
+++ b/data/raw/FormattedArchaealMetadata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="111">
   <si>
     <t>host</t>
   </si>
@@ -316,36 +316,6 @@
   </si>
   <si>
     <t>habitat_slv</t>
-  </si>
-  <si>
-    <t>agriculture</t>
-  </si>
-  <si>
-    <t>marine</t>
-  </si>
-  <si>
-    <t>surface</t>
-  </si>
-  <si>
-    <t>vertebrate</t>
-  </si>
-  <si>
-    <t>pollution</t>
-  </si>
-  <si>
-    <t>desert</t>
-  </si>
-  <si>
-    <t>fresh</t>
-  </si>
-  <si>
-    <t>root</t>
-  </si>
-  <si>
-    <t>arthopod</t>
-  </si>
-  <si>
-    <t>industrial/mining</t>
   </si>
   <si>
     <t>BI</t>
@@ -747,7 +717,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL47"/>
+  <dimension ref="A1:AE47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -852,7 +822,7 @@
         <v>98</v>
       </c>
       <c r="AE1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:31">
@@ -881,7 +851,7 @@
         <v>92</v>
       </c>
       <c r="AE2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:31">
@@ -910,7 +880,7 @@
         <v>92</v>
       </c>
       <c r="AE3" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:31">
@@ -942,7 +912,7 @@
         <v>93</v>
       </c>
       <c r="AE4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:31">
@@ -965,7 +935,7 @@
         <v>94</v>
       </c>
       <c r="AE5" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:31">
@@ -988,7 +958,7 @@
         <v>94</v>
       </c>
       <c r="AE6" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:31">
@@ -1017,7 +987,7 @@
         <v>92</v>
       </c>
       <c r="AE7" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:31">
@@ -1049,7 +1019,7 @@
         <v>93</v>
       </c>
       <c r="AE8" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:31">
@@ -1072,7 +1042,7 @@
         <v>94</v>
       </c>
       <c r="AE9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:31">
@@ -1095,7 +1065,7 @@
         <v>94</v>
       </c>
       <c r="AE10" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:31">
@@ -1127,7 +1097,7 @@
         <v>92</v>
       </c>
       <c r="AE11" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:31">
@@ -1150,7 +1120,7 @@
         <v>94</v>
       </c>
       <c r="AE12" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:31">
@@ -1182,7 +1152,7 @@
         <v>92</v>
       </c>
       <c r="AE13" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:31">
@@ -1214,7 +1184,7 @@
         <v>92</v>
       </c>
       <c r="AE14" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:31">
@@ -1237,7 +1207,7 @@
         <v>94</v>
       </c>
       <c r="AE15" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:31">
@@ -1260,7 +1230,7 @@
         <v>94</v>
       </c>
       <c r="AE16" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:31">
@@ -1292,7 +1262,7 @@
         <v>92</v>
       </c>
       <c r="AE17" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:31">
@@ -1315,7 +1285,7 @@
         <v>94</v>
       </c>
       <c r="AE18" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:31">
@@ -1347,7 +1317,7 @@
         <v>92</v>
       </c>
       <c r="AE19" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:31">
@@ -1370,7 +1340,7 @@
         <v>94</v>
       </c>
       <c r="AE20" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:31">
@@ -1402,7 +1372,7 @@
         <v>95</v>
       </c>
       <c r="AE21" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:31">
@@ -1431,7 +1401,7 @@
         <v>92</v>
       </c>
       <c r="AE22" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:31">
@@ -1454,7 +1424,7 @@
         <v>94</v>
       </c>
       <c r="AE23" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:31">
@@ -1486,7 +1456,7 @@
         <v>92</v>
       </c>
       <c r="AE24" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:31">
@@ -1518,7 +1488,7 @@
         <v>92</v>
       </c>
       <c r="AE25" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:31">
@@ -1550,7 +1520,7 @@
         <v>93</v>
       </c>
       <c r="AE26" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:31">
@@ -1582,7 +1552,7 @@
         <v>95</v>
       </c>
       <c r="AE27" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:31">
@@ -1614,7 +1584,7 @@
         <v>92</v>
       </c>
       <c r="AE28" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:31">
@@ -1637,7 +1607,7 @@
         <v>94</v>
       </c>
       <c r="AE29" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:31">
@@ -1666,7 +1636,7 @@
         <v>92</v>
       </c>
       <c r="AE30" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:31">
@@ -1689,7 +1659,7 @@
         <v>94</v>
       </c>
       <c r="AE31" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:31">
@@ -1721,10 +1691,10 @@
         <v>92</v>
       </c>
       <c r="AE32" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="33" spans="1:38">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31">
       <c r="A33">
         <v>2264867067</v>
       </c>
@@ -1750,10 +1720,10 @@
         <v>92</v>
       </c>
       <c r="AE33" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="34" spans="1:38">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31">
       <c r="A34">
         <v>2527291512</v>
       </c>
@@ -1782,10 +1752,10 @@
         <v>92</v>
       </c>
       <c r="AE34" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:38">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31">
       <c r="A35">
         <v>2264867066</v>
       </c>
@@ -1811,10 +1781,10 @@
         <v>92</v>
       </c>
       <c r="AE35" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="36" spans="1:38">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31">
       <c r="A36">
         <v>2529292698</v>
       </c>
@@ -1840,10 +1810,10 @@
         <v>96</v>
       </c>
       <c r="AE36" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:38">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31">
       <c r="A37">
         <v>2264867218</v>
       </c>
@@ -1872,10 +1842,10 @@
         <v>92</v>
       </c>
       <c r="AE37" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="38" spans="1:38">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31">
       <c r="A38">
         <v>2524614572</v>
       </c>
@@ -1895,10 +1865,10 @@
         <v>94</v>
       </c>
       <c r="AE38" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="1:38">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31">
       <c r="A39">
         <v>2527291509</v>
       </c>
@@ -1927,10 +1897,10 @@
         <v>92</v>
       </c>
       <c r="AE39" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="40" spans="1:38">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31">
       <c r="A40">
         <v>2527291506</v>
       </c>
@@ -1956,10 +1926,10 @@
         <v>92</v>
       </c>
       <c r="AE40" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="1:38">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31">
       <c r="A41">
         <v>2264867064</v>
       </c>
@@ -1988,10 +1958,10 @@
         <v>92</v>
       </c>
       <c r="AE41" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31">
       <c r="A42">
         <v>2517572170</v>
       </c>
@@ -2020,10 +1990,10 @@
         <v>95</v>
       </c>
       <c r="AE42" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:38">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31">
       <c r="A43">
         <v>2517572172</v>
       </c>
@@ -2052,10 +2022,10 @@
         <v>95</v>
       </c>
       <c r="AE43" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="44" spans="1:38">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31">
       <c r="A44">
         <v>2264867070</v>
       </c>
@@ -2081,10 +2051,10 @@
         <v>92</v>
       </c>
       <c r="AE44" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="45" spans="1:38">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31">
       <c r="A45">
         <v>2264867069</v>
       </c>
@@ -2113,10 +2083,10 @@
         <v>92</v>
       </c>
       <c r="AE45" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="46" spans="1:38">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31">
       <c r="A46">
         <v>2263328039</v>
       </c>
@@ -2127,13 +2097,13 @@
         <v>26</v>
       </c>
       <c r="N46" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="P46" t="s">
         <v>1</v>
       </c>
       <c r="S46" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="U46" t="s">
         <v>82</v>
@@ -2147,28 +2117,13 @@
         <v>93</v>
       </c>
       <c r="AC46" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="AE46" t="s">
-        <v>111</v>
-      </c>
-      <c r="AH46" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI46" t="s">
-        <v>100</v>
-      </c>
-      <c r="AJ46" t="s">
-        <v>101</v>
-      </c>
-      <c r="AK46" t="s">
-        <v>102</v>
-      </c>
-      <c r="AL46" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="47" spans="1:38">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31">
       <c r="A47">
         <v>2513237066</v>
       </c>
@@ -2179,13 +2134,13 @@
         <v>26</v>
       </c>
       <c r="N47" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="P47" t="s">
         <v>1</v>
       </c>
       <c r="S47" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="U47" t="s">
         <v>82</v>
@@ -2194,28 +2149,13 @@
         <v>87</v>
       </c>
       <c r="AB47" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="AC47" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="AE47" t="s">
-        <v>111</v>
-      </c>
-      <c r="AH47" t="s">
-        <v>104</v>
-      </c>
-      <c r="AI47" t="s">
-        <v>105</v>
-      </c>
-      <c r="AJ47" t="s">
-        <v>106</v>
-      </c>
-      <c r="AK47" t="s">
-        <v>107</v>
-      </c>
-      <c r="AL47" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>